<commit_message>
sis id generation with guid
</commit_message>
<xml_diff>
--- a/eKreta2SDS/doc/meglévő felhasználók javítása-példa.xlsx
+++ b/eKreta2SDS/doc/meglévő felhasználók javítása-példa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marto\eKreta2SDS\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EC9ED0-AA6B-4BAD-BA74-E0EC3D96BE1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D8FA86-8912-437E-A7D6-2033A41459CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="3360" windowWidth="24240" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="törzsadat" sheetId="4" r:id="rId1"/>
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC59F491-961B-481C-91DC-194EC6C64027}">
   <dimension ref="A2:C80"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -911,7 +911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0C1FDCE-AB07-43C0-8BC0-F64D8E416B6A}">
   <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AH2" sqref="AH2"/>
     </sheetView>
   </sheetViews>

</xml_diff>